<commit_message>
Completed State Level Visualisations
Former-commit-id: a4ff1f53d24994a2c4b33fa8202620bd456f6391
</commit_message>
<xml_diff>
--- a/data/non_renewables_cagr.xlsx
+++ b/data/non_renewables_cagr.xlsx
@@ -469,33 +469,33 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Brown coal</t>
+          <t>Black coal</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-3.237219697661808</v>
+        <v>-4.283866833183724</v>
       </c>
       <c r="C3" t="n">
-        <v>4597.9545</v>
+        <v>12383.7065</v>
       </c>
       <c r="D3" t="n">
-        <v>3651.935</v>
+        <v>9114.790000000001</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Black coal</t>
+          <t>Brown coal</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-4.283866833183724</v>
+        <v>-3.237219697661808</v>
       </c>
       <c r="C4" t="n">
-        <v>12383.7065</v>
+        <v>4597.9545</v>
       </c>
       <c r="D4" t="n">
-        <v>9114.790000000001</v>
+        <v>3651.935</v>
       </c>
     </row>
     <row r="5">

</xml_diff>